<commit_message>
A new file is added
</commit_message>
<xml_diff>
--- a/Tab.xlsx
+++ b/Tab.xlsx
@@ -53,7 +53,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -69,9 +69,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -109,12 +109,12 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +149,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -181,7 +181,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -336,7 +336,13 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>34563</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>